<commit_message>
Dashboard Update October I
</commit_message>
<xml_diff>
--- a/EV Growth Panama.xlsx
+++ b/EV Growth Panama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderubaldogutierrez/Documents/GitHub Repository/EV_SalesCAMEPA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFD7CDD-30E7-9C4B-83ED-31196362E802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3ACCF69-BE18-1347-BF6F-D81A8CDDD99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9380" yWindow="2220" windowWidth="20740" windowHeight="11040" xr2:uid="{734ADA49-1AB2-44E6-B14A-A5D5359A39E3}"/>
+    <workbookView xWindow="5460" yWindow="4280" windowWidth="20740" windowHeight="11040" xr2:uid="{734ADA49-1AB2-44E6-B14A-A5D5359A39E3}"/>
   </bookViews>
   <sheets>
     <sheet name="EVPanama" sheetId="1" r:id="rId1"/>

</xml_diff>